<commit_message>
move test report to AppLocator
</commit_message>
<xml_diff>
--- a/test-datas/android-test-appium-demo.xlsx
+++ b/test-datas/android-test-appium-demo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaojiewen/Documents/workspace/AppUI/test-datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28440" yWindow="500" windowWidth="22700" windowHeight="13480" tabRatio="500" activeTab="2"/>
+    <workbookView activeTab="2" tabRatio="500" windowHeight="13480" windowWidth="22700" xWindow="39340" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="配置" sheetId="6" r:id="rId1"/>
-    <sheet name="测试场景" sheetId="3" r:id="rId2"/>
-    <sheet name="主页" sheetId="2" r:id="rId3"/>
+    <sheet name="配置" r:id="rId1" sheetId="6"/>
+    <sheet name="测试场景" r:id="rId2" sheetId="3"/>
+    <sheet name="主页" r:id="rId3" sheetId="2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
@@ -35,162 +35,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="57">
   <si>
     <t>Ts_002</t>
   </si>
   <si>
     <t>定位方式</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ding'wei</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>fang'shi</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>测试数据</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>shu'ju</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>关键字</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>guan'jian'zi</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>测试结果</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>jie'guo</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>元素描述</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>yaun'su</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>miao'shu</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>测试步骤描述</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>bu'zhou</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh eb="5" sb="4">
       <t>miao'shu</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>测试步骤 ID</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>bu'zhou</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>测试集合 ID</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>ji'he</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>测试集合ID</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>ji'he</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>测试场景描述</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>chang'jing</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh eb="5" sb="4">
       <t>miao'shu</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>是否运行</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>shi'fou</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>yun'xing</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>测试结果</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>jie'guo</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>测试页面</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>ye'mian</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>元素名称</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>yuan'su</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>ming'cheng</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>等待时间（单位：s）</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>deng'dai</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>shi'jain</t>
     </rPh>
-    <rPh sb="5" eb="6">
+    <rPh eb="6" sb="5">
       <t>dan'wei</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -207,20 +207,20 @@
   </si>
   <si>
     <t>测试编号</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>bian'hao</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>测试的 sheet</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>de</t>
     </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -234,13 +234,13 @@
   </si>
   <si>
     <t>测试场景描述</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>chang'jing</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh eb="5" sb="4">
       <t>miao'shu</t>
     </rPh>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -250,30 +250,30 @@
   </si>
   <si>
     <t>应用包名</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ying'y</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>bao'ming</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>启动 Activity</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>qi'dong</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>测试应用路径</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>ying'yong</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh eb="5" sb="4">
       <t>lu'jing</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -288,20 +288,20 @@
   </si>
   <si>
     <t>显示输入名字</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>xian'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>shu'ru</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh eb="5" sb="4">
       <t>ming'zi</t>
     </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>主页</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>zhu'ye</t>
     </rPh>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -312,34 +312,34 @@
   </si>
   <si>
     <t>输入框</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>shu'ru'kuang</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>主页</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>zhu'ye</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>输入名字</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>shu'ru</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>ming'zi</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>测试名字</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>ming'zi</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -350,13 +350,13 @@
   </si>
   <si>
     <t>点击显示按钮</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>dain'ji</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>xian'shi</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh eb="5" sb="4">
       <t>an'n</t>
     </rPh>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -367,10 +367,10 @@
   </si>
   <si>
     <t>下一页按钮</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>xia'yi'ye</t>
     </rPh>
-    <rPh sb="3" eb="4">
+    <rPh eb="4" sb="3">
       <t>an'n</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -385,13 +385,13 @@
   </si>
   <si>
     <t>显示输入名字</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>xian'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>shu'ru</t>
     </rPh>
-    <rPh sb="4" eb="5">
+    <rPh eb="5" sb="4">
       <t>ming'zi</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,10 +426,10 @@
   </si>
   <si>
     <t>测试失败</t>
-    <rPh sb="0" eb="1">
+    <rPh eb="1" sb="0">
       <t>ce'shi</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh eb="3" sb="2">
       <t>shi'bai</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -452,6 +452,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -526,42 +527,42 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="常规" xfId="0"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -595,7 +596,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -613,8 +614,8 @@
       <sheetName val="Settings"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData refreshError="1" sheetId="0"/>
+      <sheetData refreshError="1" sheetId="1"/>
       <sheetData sheetId="2">
         <row r="2">
           <cell r="A2" t="str">
@@ -637,10 +638,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -675,7 +676,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="DengXian Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="DengXian Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -710,7 +711,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="DengXian" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="DengXian"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -804,21 +805,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -835,7 +836,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -887,14 +888,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -903,12 +904,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="7" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.6640625" style="7" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26.33203125" style="7" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="31.6640625" style="7" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="27.1640625" style="7" customWidth="1" collapsed="1"/>
-    <col min="6" max="16384" width="10.83203125" style="7" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="7" width="9.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="7" width="24.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="7" width="26.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="7" width="31.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="7" width="27.1640625" collapsed="true"/>
+    <col min="6" max="16384" style="7" width="10.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -928,7 +929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row ht="32" r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>47</v>
       </c>
@@ -945,7 +946,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row ht="32" r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>45</v>
       </c>
@@ -964,23 +965,23 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.1640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1020,38 +1021,38 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="D2" type="list">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.1640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.5" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.5" style="2" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.5" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="2" width="29.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row customFormat="1" ht="48" r="1" s="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
@@ -1091,7 +1092,7 @@
       <c r="M1" s="7"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row ht="32" r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>37</v>
       </c>
@@ -1131,7 +1132,7 @@
       <c r="M2" s="7"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+    <row ht="64" r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>37</v>
       </c>
@@ -1863,23 +1864,23 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="L2:L3">
-    <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule dxfId="2" operator="equal" priority="4" stopIfTrue="1" type="cellIs">
       <formula>"FAIL"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule dxfId="1" operator="equal" priority="2" stopIfTrue="1" type="cellIs">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule dxfId="0" operator="equal" priority="3" stopIfTrue="1" type="cellIs">
       <formula>FAIL</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="G2:G4" type="list">
       <formula1>"className,xpath,id,linkText,AccessibilityId,AndroidUIAutomator,iOSNsPredicate,iOSClassChain,IosUIAutomation,cssSelector"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>